<commit_message>
Test run with Costa Rica data and working
</commit_message>
<xml_diff>
--- a/out/5WErrorReport.xlsx
+++ b/out/5WErrorReport.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX19"/>
+  <dimension ref="A1:AX18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -612,75 +612,112 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pichincha</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Pitalito</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>International Organization for Migration (IOM)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Protection (Child Protection)</t>
+          <t>Food Security</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t># of food assistance facilities supported</t>
+          <t># of refugees, migrants and members of affected host communities that receive food assistance</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>HIASi</t>
+          <t>Food assistance</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Provide Venezuelan migrants and refugees who are in need of food assistance. The food assistance will be conducted in distribution of food card. The cards have different money amounts and benefitiaries are selected through an evaluation process to measure their vulnerability including gender protection concern, women-lead household, elderly women, unemployment and number of family members.</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O2">
+        <v>478</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="R2">
+        <v>9</v>
+      </c>
+      <c r="S2">
+        <v>9</v>
+      </c>
+      <c r="T2">
+        <v>9</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>3</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>2</v>
+      </c>
+      <c r="AB2">
+        <v>3</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
       </c>
       <c r="AF2" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AL2" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AM2" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -694,52 +731,52 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Atlántico</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Barranquilla</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>International Organization for Migration (IOM)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>HIASi</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2022-02</t>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Common Services (Communication)</t>
+          <t>Health</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t># of communication products published</t>
+          <t># of refugees and migrants benefiting from primary health care consultations</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>adscew</t>
+          <t>Psychological Consultation (individual)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Assist Venezuelans migrants with psychological consultation. The activity is exclusive for adult and elderly. The budget includes honorary of the Psychologists. Psychological consultation could be conducted with individual or in group.</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -747,17 +784,51 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AL3" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AW3" t="inlineStr">
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="R3">
+        <v>38</v>
+      </c>
+      <c r="S3">
+        <v>38</v>
+      </c>
+      <c r="T3">
+        <v>38</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>3</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>27</v>
+      </c>
+      <c r="AB3">
+        <v>6</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -771,12 +842,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>International Organization for Migration (IOM)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -784,11 +860,6 @@
           <t>No</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Acción y Desarrollo</t>
-        </is>
-      </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>2022-02</t>
@@ -796,53 +867,79 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Food Security</t>
+          <t>Health</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t># of refugees, migrants and members of affected host communities that are beneficiaries of rapid response productive projects (Incl. delivery of agricultural inputs, technical assistance, etc)</t>
+          <t># of refugees and migrants benefiting from primary health care consultations</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Psychological Consultation (group)</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Assist Venezuelans migrants with psychological consultation. The activity is exclusive for adult and elderly. The budget includes honorary of the Psychologists. Psychological consultation could be conducted with individual or in group.</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O4">
-        <v>6514</v>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Mobile money transfer</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="R4">
+        <v>38</v>
+      </c>
+      <c r="S4">
+        <v>38</v>
+      </c>
+      <c r="T4">
+        <v>38</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>4</v>
+      </c>
+      <c r="Z4">
+        <v>3</v>
+      </c>
+      <c r="AA4">
+        <v>24</v>
+      </c>
+      <c r="AB4">
+        <v>7</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
       </c>
       <c r="AF4" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AL4" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AR4" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -856,17 +953,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>United Nations High Commissioner for Refugees (UNHCR)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -874,40 +971,86 @@
           <t>No</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2022-01</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Health</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t># of policies and programs supported by the sector to facilitate access to national protection systems</t>
+          <t># of refugees and migrants benefiting from primary health care consultations</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Seguro médico bajo Convenio ACNUR-CCSS</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Personas venezolanas que reciben seguro médico bajo el Convenio ACNUR-CCSS</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O5">
-        <v>44</v>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AL5" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AM5" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AO5" t="inlineStr">
+          <t>No</t>
+        </is>
+      </c>
+      <c r="R5">
+        <v>1185</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -921,22 +1064,62 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>100% Diversidad y Derechos</t>
+          <t>International Organization for Migration (IOM)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Alianza VenCR</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2022-01</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Health</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t># of refugees and migrants benefiting from primary health care consultations</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Psychiatric Consultation</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Assist Venezuelans migrants who are in need of psychiatric consultation. The budget includes honorary of the Psychiatric doctors, consultation fee and psychiatric medicines.</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -944,35 +1127,46 @@
           <t>No</t>
         </is>
       </c>
-      <c r="O6">
-        <v>6514</v>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>Mobile money transfer</t>
-        </is>
-      </c>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AK6" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AL6" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AM6" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AP6" t="inlineStr">
+      <c r="R6">
+        <v>6</v>
+      </c>
+      <c r="S6">
+        <v>6</v>
+      </c>
+      <c r="T6">
+        <v>6</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>4</v>
+      </c>
+      <c r="AB6">
+        <v>2</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -986,47 +1180,57 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>United Nations High Commissioner for Refugees (UNHCR)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Fundación Mujer</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2022-08</t>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Common Services (Communication)</t>
+          <t>Integration</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t># of views to the R4V newsletter</t>
+          <t># of refugees, migrants &amp; host community members reached with financial inclusion activities</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>tuyjy</t>
+          <t>Capacitación Base o Empoderamiento general</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Entrenamiento en habilidades blandas, empoderamiento legal y educación financiera que favorezca la integración en el país</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1039,10 +1243,34 @@
           <t>No</t>
         </is>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="AW7" t="inlineStr">
+      <c r="R7">
+        <v>12</v>
+      </c>
+      <c r="S7">
+        <v>12</v>
+      </c>
+      <c r="T7">
+        <v>12</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>9</v>
+      </c>
+      <c r="AB7">
+        <v>3</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -1056,47 +1284,57 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>United Nations High Commissioner for Refugees (UNHCR)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Fundación Mujer</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2022-09</t>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Common Services (Communication)</t>
+          <t>Integration</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t># of views to the R4V newsletter</t>
+          <t># of refugees, migrants &amp; host community members receiving support activities/interventions enabling them to access or to keep a job</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>tujuyt</t>
+          <t>Diagnóstico de Medios de Vida</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Identificar perfil profesional-ocupacional, el estado de títulos e información del proceso de homologación o convalidación del mismo</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1109,7 +1347,34 @@
           <t>No</t>
         </is>
       </c>
-      <c r="AW8" t="inlineStr">
+      <c r="R8">
+        <v>24</v>
+      </c>
+      <c r="S8">
+        <v>24</v>
+      </c>
+      <c r="T8">
+        <v>24</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>17</v>
+      </c>
+      <c r="AB8">
+        <v>6</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AF8" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -1123,47 +1388,57 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>United Nations High Commissioner for Refugees (UNHCR)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>RET International</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2022-10</t>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Common Services (Communication)</t>
+          <t>Multipurpose Cash Assistance (MPC)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t># of views to the R4V newsletter</t>
+          <t># of individuals benefitting from multipurpose cash transfers (MPC)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>tujuyt</t>
+          <t>IMAS</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>PdI valorada en IMAS</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1173,32 +1448,81 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="Q9">
-        <v>3</v>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O9">
+        <v>100</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Bank transfer</t>
+        </is>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+      <c r="AX9" t="inlineStr">
+        <is>
+          <t>Please review activity</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>United Nations High Commissioner for Refugees (UNHCR)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1208,7 +1532,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2022-11</t>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1221,6 +1545,21 @@
           <t># of individuals benefitting from multipurpose cash transfers (MPC)</t>
         </is>
       </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Multi-purpose cash assistance</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>MPCA for basic needs based on socioeconomic vulnerability</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1228,39 +1567,48 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O10">
+        <v>3677.18</v>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Other electronic cash mechanisms</t>
         </is>
       </c>
       <c r="R10">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="S10">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="T10">
+        <v>25</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
         <v>5</v>
       </c>
-      <c r="U10">
-        <v>5</v>
+      <c r="Z10">
+        <v>3</v>
       </c>
       <c r="AA10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AB10">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AC10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AD10">
-        <v>1</v>
-      </c>
-      <c r="AL10" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AQ10" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="AF10" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -1274,42 +1622,57 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>United Nations High Commissioner for Refugees (UNHCR)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>RET International</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2022-12</t>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Multipurpose Cash Assistance (MPC)</t>
+          <t>Protection (GBV)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t># of individuals benefitting from multipurpose cash transfers (MPC)</t>
+          <t># of refugees, migrants and affected host community members reached with GBV prevention, mitigation and response activities</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>VBG</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>PdI valorada para acceso a la justicia o redes de apoyo VBG</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1319,37 +1682,52 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O11">
-        <v>6514</v>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>Mobile money transfer</t>
-        </is>
+        <v>0</v>
       </c>
       <c r="R11">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="S11">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="T11">
-        <v>50</v>
-      </c>
-      <c r="AL11" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AS11" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AU11" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>2</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AF11" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -1363,27 +1741,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>United Nations High Commissioner for Refugees (UNHCR)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>RET International</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1393,12 +1771,27 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Multipurpose Cash Assistance (MPC)</t>
+          <t>Protection (General)</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t># of individuals benefitting from multipurpose cash transfers (MPC)</t>
+          <t># of refugees and migrants who received protection-related assistance and specialized services</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Psicosocial</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>PdI atendida en psicosocial</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1408,40 +1801,52 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O12">
-        <v>6515</v>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>Mobile money transfer</t>
-        </is>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="S12">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="T12">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="U12">
-        <v>3</v>
-      </c>
-      <c r="AL12" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AT12" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AU12" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>5</v>
+      </c>
+      <c r="AB12">
+        <v>1</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AF12" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -1455,42 +1860,52 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>United Nations High Commissioner for Refugees (UNHCR)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>HIAS</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2022-02</t>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Multipurpose Cash Assistance (MPC)</t>
+          <t>Protection (General)</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t># of individuals benefitting from multipurpose cash transfers (MPC)</t>
+          <t># of refugees and migrants who received protection-related assistance and specialized services</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Brindar información, asesoría y representación legal en materia del procedimiento para la determinación de la condición de persona refugiada a la población solicitante de refugio y refugiada</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -1500,38 +1915,37 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O13">
-        <v>6516</v>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>Mobile money transfer</t>
+          <t>No</t>
         </is>
       </c>
       <c r="R13">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="S13">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="T13">
-        <v>33</v>
-      </c>
-      <c r="U13">
-        <v>7</v>
+        <v>45</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>24</v>
+      </c>
+      <c r="AB13">
+        <v>21</v>
       </c>
       <c r="AC13">
-        <v>12</v>
-      </c>
-      <c r="AL13" t="inlineStr">
-        <is>
-          <t>Review</t>
-        </is>
-      </c>
-      <c r="AU13" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AF13" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -1545,47 +1959,57 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>United Nations High Commissioner for Refugees (UNHCR)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>RET International</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2022-03</t>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>WASH</t>
+          <t>Protection (General)</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t># de instalaciones WASH (comunitarias/pública) mejoradas o establecidas</t>
+          <t># of refugees and migrants who received protection-related assistance and specialized services</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>tujuyt</t>
+          <t>Protección gestion de casos</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>PdI valorada para necesidades de protección</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1598,29 +2022,73 @@
           <t>No</t>
         </is>
       </c>
-      <c r="Q14">
-        <v>4</v>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+      <c r="AX14" t="inlineStr">
+        <is>
+          <t>Please review activity</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>International Organization for Migration (IOM)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1630,22 +2098,32 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2022-04</t>
+          <t>2022-02</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>WASH</t>
+          <t>Protection (General)</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t># de instalaciones WASH (comunitarias/pública) mejoradas o establecidas</t>
+          <t># of refugees and migrants who received protection-related assistance and specialized services</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>tujuyt</t>
+          <t>Legal Assistance</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Refugees and migrants who receive immigration legal assistance. The budget of this activity includes staff fees, migratory legal consultation sessions in San José and other regions outside the Central Valley.</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1658,7 +2136,46 @@
           <t>No</t>
         </is>
       </c>
-      <c r="AW15" t="inlineStr">
+      <c r="R15">
+        <v>72</v>
+      </c>
+      <c r="S15">
+        <v>72</v>
+      </c>
+      <c r="T15">
+        <v>72</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>48</v>
+      </c>
+      <c r="AB15">
+        <v>23</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AF15" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -1672,47 +2189,57 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>International Organization for Migration (IOM)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Alianza VenCR</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2022-05</t>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Food Security</t>
+          <t>Shelter</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t># of individuals working with refugees,  migrants and affected host communities trained in food security and/or the provision of food services and assistance</t>
+          <t># of refugees and migrants hosted in temporary supported collective shelter solutions</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>tujuyt</t>
+          <t>Temporary Accommodation</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Provide Venezuelan refugees and migrants with temporary accommodation in forms of individual shelter. Each beneficiary will be given maximum 10 nights at temporary accommodation. IOM Costa Rica has an agreement with two shelter houses:"Casa de acogida Ciudad de Paz" and "Casa Ridway". Each migrant has the possibility of staying in a private room. Each night costs $14.</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1726,28 +2253,69 @@
         </is>
       </c>
       <c r="R16">
-        <v>44</v>
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>Review</t>
+        </is>
+      </c>
+      <c r="AX16" t="inlineStr">
+        <is>
+          <t>Please review activity</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>International Organization for Migration (IOM)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1757,22 +2325,32 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2022-06</t>
+          <t>2022-01</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Food Security</t>
+          <t>WASH</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t># of individuals working with refugees,  migrants and affected host communities trained in food security and/or the provision of food services and assistance</t>
+          <t># of refugees and migrants and/or host communities provided with appropriate hygiene supplies and services (messages, items, facilities) including women and girls provided with menstrual hygiene management services</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>tujuyt</t>
+          <t>Diapers</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Personal hygiene kits - ADG (age gender and diversity sensitive). The activity tries to cover the need of refugees and migrants from Venezuela in diapers for their babies</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1785,7 +2363,46 @@
           <t>No</t>
         </is>
       </c>
-      <c r="AV17" t="inlineStr">
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AF17" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -1799,22 +2416,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Acción y Desarrollo</t>
+          <t>International Organization for Migration (IOM)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1824,22 +2436,32 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2022-07</t>
+          <t>2022-02</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Education</t>
+          <t>WASH</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t># of information, awareness-raising, promotion and dissemination activities on the importance of the Right to Education, availability and quality of education implemented</t>
+          <t># of refugees and migrants and/or host communities provided with appropriate hygiene supplies and services (messages, items, facilities) including women and girls provided with menstrual hygiene management services</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>tujuyt</t>
+          <t>Hygiene Kitts</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Refugees and migrants from Venezuela that are supported with hygiene kitts. This assistance is designed to ensure that Venezuelans receive a basic hygiene kitt and is not designed to be CBI, given that migrants prefer to spend cash assistance in other needs such as food. The activity is aimed to respond to COVID-19 situation due to the hygiene elements that are included in the kitt.</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1852,7 +2474,46 @@
           <t>No</t>
         </is>
       </c>
-      <c r="AW18" t="inlineStr">
+      <c r="R18">
+        <v>9</v>
+      </c>
+      <c r="S18">
+        <v>9</v>
+      </c>
+      <c r="T18">
+        <v>9</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>3</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>2</v>
+      </c>
+      <c r="AB18">
+        <v>3</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AF18" t="inlineStr">
         <is>
           <t>Review</t>
         </is>
@@ -1861,66 +2522,6 @@
         <is>
           <t>Please review activity</t>
         </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Colombia</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Antioquia</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Alejandría</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Acción y Desarrollo</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2022-08</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Education</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t># of information, awareness-raising, promotion and dissemination activities on the importance of the Right to Education, availability and quality of education implemented</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>tujuyt</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="Q19">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>